<commit_message>
Added alarm for status change and 30-min poor alert with sound
</commit_message>
<xml_diff>
--- a/server/data/locations.xlsx
+++ b/server/data/locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\connect\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F0A06B-07BE-46BC-A0BF-6EB8C81DF01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BC6379-D198-4D48-884A-268DA580DBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="218">
   <si>
     <t>Location Name</t>
   </si>
@@ -631,34 +631,49 @@
     <t>172.24.196.86</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>8.8.8.8</t>
   </si>
   <si>
     <t>1.1.1.1</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>203.0.113.1</t>
-  </si>
-  <si>
     <t>9.9.9.9</t>
   </si>
   <si>
-    <t>127.0.0.1</t>
-  </si>
-  <si>
     <t>8.8.4.4</t>
   </si>
   <si>
-    <t>Banglore</t>
+    <t>Google DNS</t>
+  </si>
+  <si>
+    <t>Cloudflare DNS</t>
+  </si>
+  <si>
+    <t>1.0.0.1</t>
+  </si>
+  <si>
+    <t>Quad9</t>
+  </si>
+  <si>
+    <t>149.112.112.112</t>
+  </si>
+  <si>
+    <t>OpenDNS</t>
+  </si>
+  <si>
+    <t>208.67.222.222</t>
+  </si>
+  <si>
+    <t>208.67.220.220</t>
+  </si>
+  <si>
+    <t>Comodo DNS</t>
+  </si>
+  <si>
+    <t>8.26.56.26</t>
+  </si>
+  <si>
+    <t>8.20.247.20</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2071,30 +2086,21 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C52" t="s">
         <v>206</v>
       </c>
-      <c r="D52" t="s">
-        <v>206</v>
-      </c>
       <c r="E52" t="s">
-        <v>205</v>
-      </c>
-      <c r="F52" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>207</v>
-      </c>
-      <c r="B53" t="s">
         <v>208</v>
+      </c>
+      <c r="C53" t="s">
+        <v>204</v>
       </c>
       <c r="E53" t="s">
         <v>209</v>
@@ -2102,13 +2108,35 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>212</v>
-      </c>
-      <c r="B54" t="s">
         <v>210</v>
+      </c>
+      <c r="C54" t="s">
+        <v>205</v>
       </c>
       <c r="E54" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" t="s">
+        <v>213</v>
+      </c>
+      <c r="E55" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>215</v>
+      </c>
+      <c r="C56" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>